<commit_message>
fixed data glitch and visual minus final path is done
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\368 final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\PycharmProjects\CSE368_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568D1D67-E915-47F4-BD55-E10CC29662AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DF879C-4706-4844-9356-E5F7715A9D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F81B381-2B76-4613-A2B4-2596578C5B47}"/>
   </bookViews>
@@ -2940,9 +2940,6 @@
     <t>IA, NE, MN, MO</t>
   </si>
   <si>
-    <t>Iowa City, Lincoln, Minneapolis, Kasas City</t>
-  </si>
-  <si>
     <t>Columbia, Lawrence, Des Moines, St. Joseph, Wichita</t>
   </si>
   <si>
@@ -3898,6 +3895,9 @@
   </si>
   <si>
     <t>166666, 107137, 33901, 38381</t>
+  </si>
+  <si>
+    <t>Iowa City, Lincoln, Minneapolis, Kansas City</t>
   </si>
 </sst>
 </file>
@@ -3956,16 +3956,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4303,8 +4299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444078F1-5048-4592-B562-D8390E91F891}">
   <dimension ref="A1:H316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D200" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F215" sqref="F215"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4341,7 +4337,7 @@
       <c r="G1" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4367,8 +4363,8 @@
       <c r="G2" t="s">
         <v>727</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>974</v>
+      <c r="H2" t="s">
+        <v>973</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -4393,8 +4389,8 @@
       <c r="G3" t="s">
         <v>727</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>975</v>
+      <c r="H3" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -4419,8 +4415,8 @@
       <c r="G4" t="s">
         <v>728</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>976</v>
+      <c r="H4" t="s">
+        <v>975</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4445,8 +4441,8 @@
       <c r="G5" t="s">
         <v>729</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>977</v>
+      <c r="H5" t="s">
+        <v>976</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4471,8 +4467,8 @@
       <c r="G6" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>978</v>
+      <c r="H6" t="s">
+        <v>977</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -4497,8 +4493,8 @@
       <c r="G7" t="s">
         <v>730</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>979</v>
+      <c r="H7" t="s">
+        <v>978</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4523,8 +4519,8 @@
       <c r="G8" t="s">
         <v>731</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>980</v>
+      <c r="H8" t="s">
+        <v>979</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -4549,8 +4545,8 @@
       <c r="G9" t="s">
         <v>732</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>981</v>
+      <c r="H9" t="s">
+        <v>980</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -4575,8 +4571,8 @@
       <c r="G10" t="s">
         <v>733</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>982</v>
+      <c r="H10" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -4601,8 +4597,8 @@
       <c r="G11" t="s">
         <v>734</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>983</v>
+      <c r="H11" t="s">
+        <v>982</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -4627,8 +4623,8 @@
       <c r="G12" t="s">
         <v>735</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>984</v>
+      <c r="H12" t="s">
+        <v>983</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -4653,8 +4649,8 @@
       <c r="G13" t="s">
         <v>736</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>985</v>
+      <c r="H13" t="s">
+        <v>984</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -4679,8 +4675,8 @@
       <c r="G14" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>986</v>
+      <c r="H14" t="s">
+        <v>985</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -4705,8 +4701,8 @@
       <c r="G15" t="s">
         <v>737</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>987</v>
+      <c r="H15" t="s">
+        <v>986</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -4731,8 +4727,8 @@
       <c r="G16" t="s">
         <v>738</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>988</v>
+      <c r="H16" t="s">
+        <v>987</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -4757,8 +4753,8 @@
       <c r="G17" t="s">
         <v>739</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>989</v>
+      <c r="H17" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -4783,8 +4779,8 @@
       <c r="G18" t="s">
         <v>740</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>990</v>
+      <c r="H18" t="s">
+        <v>989</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -4809,8 +4805,8 @@
       <c r="G19" t="s">
         <v>733</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>991</v>
+      <c r="H19" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -4835,8 +4831,8 @@
       <c r="G20" t="s">
         <v>740</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>992</v>
+      <c r="H20" t="s">
+        <v>991</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -4861,8 +4857,8 @@
       <c r="G21" t="s">
         <v>741</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>993</v>
+      <c r="H21" t="s">
+        <v>992</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -4887,8 +4883,8 @@
       <c r="G22" t="s">
         <v>742</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>994</v>
+      <c r="H22" t="s">
+        <v>993</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -4913,8 +4909,8 @@
       <c r="G23" t="s">
         <v>740</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>995</v>
+      <c r="H23" t="s">
+        <v>994</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -4939,8 +4935,8 @@
       <c r="G24" t="s">
         <v>743</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>996</v>
+      <c r="H24" t="s">
+        <v>995</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -4965,8 +4961,8 @@
       <c r="G25" t="s">
         <v>744</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>997</v>
+      <c r="H25" t="s">
+        <v>996</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -4991,8 +4987,8 @@
       <c r="G26" t="s">
         <v>745</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>998</v>
+      <c r="H26" t="s">
+        <v>997</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -5017,8 +5013,8 @@
       <c r="G27" t="s">
         <v>742</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>999</v>
+      <c r="H27" t="s">
+        <v>998</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -5043,8 +5039,8 @@
       <c r="G28" t="s">
         <v>40</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>1000</v>
+      <c r="H28" t="s">
+        <v>999</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -5069,8 +5065,8 @@
       <c r="G29" t="s">
         <v>740</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>1001</v>
+      <c r="H29" t="s">
+        <v>1000</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -5095,8 +5091,8 @@
       <c r="G30" t="s">
         <v>740</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>1002</v>
+      <c r="H30" t="s">
+        <v>1001</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -5121,8 +5117,8 @@
       <c r="G31" t="s">
         <v>740</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>1003</v>
+      <c r="H31" t="s">
+        <v>1002</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -5147,8 +5143,8 @@
       <c r="G32" t="s">
         <v>740</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>1004</v>
+      <c r="H32" t="s">
+        <v>1003</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -5173,8 +5169,8 @@
       <c r="G33" t="s">
         <v>740</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>1005</v>
+      <c r="H33" t="s">
+        <v>1004</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -5199,8 +5195,8 @@
       <c r="G34" t="s">
         <v>746</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>1006</v>
+      <c r="H34" t="s">
+        <v>1005</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -5225,8 +5221,8 @@
       <c r="G35" t="s">
         <v>747</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>1007</v>
+      <c r="H35" t="s">
+        <v>1006</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -5251,8 +5247,8 @@
       <c r="G36" t="s">
         <v>748</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>1008</v>
+      <c r="H36" t="s">
+        <v>1007</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -5277,8 +5273,8 @@
       <c r="G37" t="s">
         <v>749</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>1009</v>
+      <c r="H37" t="s">
+        <v>1008</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -5303,8 +5299,8 @@
       <c r="G38" t="s">
         <v>47</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>1010</v>
+      <c r="H38" t="s">
+        <v>1009</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -5329,8 +5325,8 @@
       <c r="G39" t="s">
         <v>750</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>1011</v>
+      <c r="H39" t="s">
+        <v>1010</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -5355,8 +5351,8 @@
       <c r="G40" t="s">
         <v>751</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>1012</v>
+      <c r="H40" t="s">
+        <v>1011</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -5381,8 +5377,8 @@
       <c r="G41" t="s">
         <v>752</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>1013</v>
+      <c r="H41" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -5407,8 +5403,8 @@
       <c r="G42" t="s">
         <v>753</v>
       </c>
-      <c r="H42" s="3" t="s">
-        <v>1014</v>
+      <c r="H42" t="s">
+        <v>1013</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -5433,8 +5429,8 @@
       <c r="G43" t="s">
         <v>754</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>1015</v>
+      <c r="H43" t="s">
+        <v>1014</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -5459,8 +5455,8 @@
       <c r="G44" t="s">
         <v>755</v>
       </c>
-      <c r="H44" s="3" t="s">
-        <v>1016</v>
+      <c r="H44" t="s">
+        <v>1015</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -5485,8 +5481,8 @@
       <c r="G45" t="s">
         <v>756</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>1017</v>
+      <c r="H45" t="s">
+        <v>1016</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -5511,8 +5507,8 @@
       <c r="G46" t="s">
         <v>757</v>
       </c>
-      <c r="H46" s="3" t="s">
-        <v>1018</v>
+      <c r="H46" t="s">
+        <v>1017</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -5537,8 +5533,8 @@
       <c r="G47" t="s">
         <v>897</v>
       </c>
-      <c r="H47" s="3" t="s">
-        <v>1019</v>
+      <c r="H47" t="s">
+        <v>1018</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -5563,8 +5559,8 @@
       <c r="G48" t="s">
         <v>758</v>
       </c>
-      <c r="H48" s="3" t="s">
-        <v>1020</v>
+      <c r="H48" t="s">
+        <v>1019</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
@@ -5589,8 +5585,8 @@
       <c r="G49" t="s">
         <v>758</v>
       </c>
-      <c r="H49" s="3" t="s">
-        <v>1021</v>
+      <c r="H49" t="s">
+        <v>1020</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -5615,8 +5611,8 @@
       <c r="G50" t="s">
         <v>758</v>
       </c>
-      <c r="H50" s="3" t="s">
-        <v>1022</v>
+      <c r="H50" t="s">
+        <v>1021</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -5641,8 +5637,8 @@
       <c r="G51" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="3" t="s">
-        <v>1023</v>
+      <c r="H51" t="s">
+        <v>1022</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -5667,8 +5663,8 @@
       <c r="G52" t="s">
         <v>758</v>
       </c>
-      <c r="H52" s="3" t="s">
-        <v>1024</v>
+      <c r="H52" t="s">
+        <v>1023</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -5693,8 +5689,8 @@
       <c r="G53" t="s">
         <v>758</v>
       </c>
-      <c r="H53" s="3" t="s">
-        <v>1025</v>
+      <c r="H53" t="s">
+        <v>1024</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -5719,8 +5715,8 @@
       <c r="G54" t="s">
         <v>759</v>
       </c>
-      <c r="H54" s="3" t="s">
-        <v>1026</v>
+      <c r="H54" t="s">
+        <v>1025</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -5745,8 +5741,8 @@
       <c r="G55" t="s">
         <v>760</v>
       </c>
-      <c r="H55" s="3" t="s">
-        <v>1027</v>
+      <c r="H55" t="s">
+        <v>1026</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -5771,8 +5767,8 @@
       <c r="G56" t="s">
         <v>761</v>
       </c>
-      <c r="H56" s="3" t="s">
-        <v>1028</v>
+      <c r="H56" t="s">
+        <v>1027</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -5797,8 +5793,8 @@
       <c r="G57" t="s">
         <v>758</v>
       </c>
-      <c r="H57" s="3" t="s">
-        <v>1029</v>
+      <c r="H57" t="s">
+        <v>1028</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
@@ -5823,8 +5819,8 @@
       <c r="G58" t="s">
         <v>758</v>
       </c>
-      <c r="H58" s="3" t="s">
-        <v>1030</v>
+      <c r="H58" t="s">
+        <v>1029</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
@@ -5849,8 +5845,8 @@
       <c r="G59" t="s">
         <v>82</v>
       </c>
-      <c r="H59" s="3" t="s">
-        <v>1031</v>
+      <c r="H59" t="s">
+        <v>1030</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -5875,8 +5871,8 @@
       <c r="G60" t="s">
         <v>758</v>
       </c>
-      <c r="H60" s="3" t="s">
-        <v>1032</v>
+      <c r="H60" t="s">
+        <v>1031</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
@@ -5901,8 +5897,8 @@
       <c r="G61" t="s">
         <v>758</v>
       </c>
-      <c r="H61" s="3" t="s">
-        <v>1033</v>
+      <c r="H61" t="s">
+        <v>1032</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -5927,8 +5923,8 @@
       <c r="G62" t="s">
         <v>758</v>
       </c>
-      <c r="H62" s="3" t="s">
-        <v>1034</v>
+      <c r="H62" t="s">
+        <v>1033</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
@@ -5953,8 +5949,8 @@
       <c r="G63" t="s">
         <v>758</v>
       </c>
-      <c r="H63" s="3" t="s">
-        <v>1035</v>
+      <c r="H63" t="s">
+        <v>1034</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
@@ -5979,8 +5975,8 @@
       <c r="G64" t="s">
         <v>762</v>
       </c>
-      <c r="H64" s="3" t="s">
-        <v>1036</v>
+      <c r="H64" t="s">
+        <v>1035</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -6005,8 +6001,8 @@
       <c r="G65" t="s">
         <v>758</v>
       </c>
-      <c r="H65" s="3" t="s">
-        <v>1037</v>
+      <c r="H65" t="s">
+        <v>1036</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
@@ -6031,8 +6027,8 @@
       <c r="G66" t="s">
         <v>758</v>
       </c>
-      <c r="H66" s="3" t="s">
-        <v>1038</v>
+      <c r="H66" t="s">
+        <v>1037</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
@@ -6057,8 +6053,8 @@
       <c r="G67" t="s">
         <v>758</v>
       </c>
-      <c r="H67" s="3" t="s">
-        <v>1039</v>
+      <c r="H67" t="s">
+        <v>1038</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -6083,8 +6079,8 @@
       <c r="G68" t="s">
         <v>759</v>
       </c>
-      <c r="H68" s="3" t="s">
-        <v>1040</v>
+      <c r="H68" t="s">
+        <v>1039</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -6109,8 +6105,8 @@
       <c r="G69" t="s">
         <v>758</v>
       </c>
-      <c r="H69" s="3" t="s">
-        <v>1041</v>
+      <c r="H69" t="s">
+        <v>1040</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -6135,8 +6131,8 @@
       <c r="G70" t="s">
         <v>758</v>
       </c>
-      <c r="H70" s="3" t="s">
-        <v>1042</v>
+      <c r="H70" t="s">
+        <v>1041</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
@@ -6161,8 +6157,8 @@
       <c r="G71" t="s">
         <v>763</v>
       </c>
-      <c r="H71" s="3" t="s">
-        <v>1043</v>
+      <c r="H71" t="s">
+        <v>1042</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
@@ -6187,8 +6183,8 @@
       <c r="G72" t="s">
         <v>764</v>
       </c>
-      <c r="H72" s="3" t="s">
-        <v>1044</v>
+      <c r="H72" t="s">
+        <v>1043</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
@@ -6213,8 +6209,8 @@
       <c r="G73" t="s">
         <v>760</v>
       </c>
-      <c r="H73" s="3" t="s">
-        <v>1045</v>
+      <c r="H73" t="s">
+        <v>1044</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
@@ -6239,8 +6235,8 @@
       <c r="G74" t="s">
         <v>765</v>
       </c>
-      <c r="H74" s="3" t="s">
-        <v>1046</v>
+      <c r="H74" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
@@ -6265,8 +6261,8 @@
       <c r="G75" t="s">
         <v>766</v>
       </c>
-      <c r="H75" s="3" t="s">
-        <v>1047</v>
+      <c r="H75" t="s">
+        <v>1046</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
@@ -6291,8 +6287,8 @@
       <c r="G76" t="s">
         <v>767</v>
       </c>
-      <c r="H76" s="3" t="s">
-        <v>1048</v>
+      <c r="H76" t="s">
+        <v>1047</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
@@ -6317,8 +6313,8 @@
       <c r="G77" t="s">
         <v>760</v>
       </c>
-      <c r="H77" s="3" t="s">
-        <v>1049</v>
+      <c r="H77" t="s">
+        <v>1048</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
@@ -6343,8 +6339,8 @@
       <c r="G78" t="s">
         <v>768</v>
       </c>
-      <c r="H78" s="3" t="s">
-        <v>1050</v>
+      <c r="H78" t="s">
+        <v>1049</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
@@ -6369,8 +6365,8 @@
       <c r="G79" t="s">
         <v>769</v>
       </c>
-      <c r="H79" s="3" t="s">
-        <v>1051</v>
+      <c r="H79" t="s">
+        <v>1050</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
@@ -6395,8 +6391,8 @@
       <c r="G80" t="s">
         <v>770</v>
       </c>
-      <c r="H80" s="3" t="s">
-        <v>1052</v>
+      <c r="H80" t="s">
+        <v>1051</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
@@ -6421,8 +6417,8 @@
       <c r="G81" t="s">
         <v>771</v>
       </c>
-      <c r="H81" s="3" t="s">
-        <v>1053</v>
+      <c r="H81" t="s">
+        <v>1052</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
@@ -6447,8 +6443,8 @@
       <c r="G82" t="s">
         <v>772</v>
       </c>
-      <c r="H82" s="3" t="s">
-        <v>1054</v>
+      <c r="H82" t="s">
+        <v>1053</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
@@ -6473,8 +6469,8 @@
       <c r="G83" t="s">
         <v>769</v>
       </c>
-      <c r="H83" s="3" t="s">
-        <v>1055</v>
+      <c r="H83" t="s">
+        <v>1054</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
@@ -6499,8 +6495,8 @@
       <c r="G84" t="s">
         <v>773</v>
       </c>
-      <c r="H84" s="3" t="s">
-        <v>1056</v>
+      <c r="H84" t="s">
+        <v>1055</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
@@ -6525,8 +6521,8 @@
       <c r="G85" t="s">
         <v>774</v>
       </c>
-      <c r="H85" s="3" t="s">
-        <v>1057</v>
+      <c r="H85" t="s">
+        <v>1056</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -6551,8 +6547,8 @@
       <c r="G86" t="s">
         <v>775</v>
       </c>
-      <c r="H86" s="3" t="s">
-        <v>1058</v>
+      <c r="H86" t="s">
+        <v>1057</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
@@ -6577,8 +6573,8 @@
       <c r="G87" t="s">
         <v>776</v>
       </c>
-      <c r="H87" s="3" t="s">
-        <v>1059</v>
+      <c r="H87" t="s">
+        <v>1058</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
@@ -6603,8 +6599,8 @@
       <c r="G88" t="s">
         <v>99</v>
       </c>
-      <c r="H88" s="3" t="s">
-        <v>1060</v>
+      <c r="H88" t="s">
+        <v>1059</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
@@ -6629,8 +6625,8 @@
       <c r="G89" t="s">
         <v>99</v>
       </c>
-      <c r="H89" s="3" t="s">
-        <v>1061</v>
+      <c r="H89" t="s">
+        <v>1060</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
@@ -6655,8 +6651,8 @@
       <c r="G90" t="s">
         <v>777</v>
       </c>
-      <c r="H90" s="3" t="s">
-        <v>1062</v>
+      <c r="H90" t="s">
+        <v>1061</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
@@ -6681,8 +6677,8 @@
       <c r="G91" t="s">
         <v>778</v>
       </c>
-      <c r="H91" s="3" t="s">
-        <v>1063</v>
+      <c r="H91" t="s">
+        <v>1062</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
@@ -6707,8 +6703,8 @@
       <c r="G92" t="s">
         <v>779</v>
       </c>
-      <c r="H92" s="3" t="s">
-        <v>1064</v>
+      <c r="H92" t="s">
+        <v>1063</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
@@ -6733,8 +6729,8 @@
       <c r="G93" t="s">
         <v>963</v>
       </c>
-      <c r="H93" s="3" t="s">
-        <v>1065</v>
+      <c r="H93" t="s">
+        <v>1064</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
@@ -6759,8 +6755,8 @@
       <c r="G94" t="s">
         <v>780</v>
       </c>
-      <c r="H94" s="3" t="s">
-        <v>1066</v>
+      <c r="H94" t="s">
+        <v>1065</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
@@ -6785,8 +6781,8 @@
       <c r="G95" t="s">
         <v>780</v>
       </c>
-      <c r="H95" s="3" t="s">
-        <v>1067</v>
+      <c r="H95" t="s">
+        <v>1066</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
@@ -6811,8 +6807,8 @@
       <c r="G96" t="s">
         <v>781</v>
       </c>
-      <c r="H96" s="3" t="s">
-        <v>1068</v>
+      <c r="H96" t="s">
+        <v>1067</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
@@ -6837,8 +6833,8 @@
       <c r="G97" t="s">
         <v>782</v>
       </c>
-      <c r="H97" s="3" t="s">
-        <v>1069</v>
+      <c r="H97" t="s">
+        <v>1068</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
@@ -6863,8 +6859,8 @@
       <c r="G98" t="s">
         <v>118</v>
       </c>
-      <c r="H98" s="3" t="s">
-        <v>1070</v>
+      <c r="H98" t="s">
+        <v>1069</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
@@ -6889,8 +6885,8 @@
       <c r="G99" t="s">
         <v>783</v>
       </c>
-      <c r="H99" s="3" t="s">
-        <v>1071</v>
+      <c r="H99" t="s">
+        <v>1070</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
@@ -6915,8 +6911,8 @@
       <c r="G100" t="s">
         <v>911</v>
       </c>
-      <c r="H100" s="3" t="s">
-        <v>1072</v>
+      <c r="H100" t="s">
+        <v>1071</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
@@ -6941,8 +6937,8 @@
       <c r="G101" t="s">
         <v>776</v>
       </c>
-      <c r="H101" s="3" t="s">
-        <v>1073</v>
+      <c r="H101" t="s">
+        <v>1072</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
@@ -6967,8 +6963,8 @@
       <c r="G102" t="s">
         <v>784</v>
       </c>
-      <c r="H102" s="3" t="s">
-        <v>1074</v>
+      <c r="H102" t="s">
+        <v>1073</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
@@ -6993,8 +6989,8 @@
       <c r="G103" t="s">
         <v>776</v>
       </c>
-      <c r="H103" s="3" t="s">
-        <v>1075</v>
+      <c r="H103" t="s">
+        <v>1074</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
@@ -7019,8 +7015,8 @@
       <c r="G104" t="s">
         <v>785</v>
       </c>
-      <c r="H104" s="3" t="s">
-        <v>1076</v>
+      <c r="H104" t="s">
+        <v>1075</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
@@ -7045,8 +7041,8 @@
       <c r="G105" t="s">
         <v>786</v>
       </c>
-      <c r="H105" s="3" t="s">
-        <v>1077</v>
+      <c r="H105" t="s">
+        <v>1076</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
@@ -7066,13 +7062,13 @@
         <v>391</v>
       </c>
       <c r="F106" t="s">
-        <v>971</v>
+        <v>1290</v>
       </c>
       <c r="G106" t="s">
         <v>970</v>
       </c>
-      <c r="H106" s="3" t="s">
-        <v>1078</v>
+      <c r="H106" t="s">
+        <v>1077</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
@@ -7097,8 +7093,8 @@
       <c r="G107" t="s">
         <v>787</v>
       </c>
-      <c r="H107" s="3" t="s">
-        <v>1079</v>
+      <c r="H107" t="s">
+        <v>1078</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
@@ -7123,8 +7119,8 @@
       <c r="G108" t="s">
         <v>788</v>
       </c>
-      <c r="H108" s="3" t="s">
-        <v>1080</v>
+      <c r="H108" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
@@ -7149,8 +7145,8 @@
       <c r="G109" t="s">
         <v>789</v>
       </c>
-      <c r="H109" s="3" t="s">
-        <v>1081</v>
+      <c r="H109" t="s">
+        <v>1080</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
@@ -7175,8 +7171,8 @@
       <c r="G110" t="s">
         <v>790</v>
       </c>
-      <c r="H110" s="3" t="s">
-        <v>1082</v>
+      <c r="H110" t="s">
+        <v>1081</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
@@ -7201,8 +7197,8 @@
       <c r="G111" t="s">
         <v>791</v>
       </c>
-      <c r="H111" s="3" t="s">
-        <v>1083</v>
+      <c r="H111" t="s">
+        <v>1082</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
@@ -7227,8 +7223,8 @@
       <c r="G112" t="s">
         <v>792</v>
       </c>
-      <c r="H112" s="3" t="s">
-        <v>1084</v>
+      <c r="H112" t="s">
+        <v>1083</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
@@ -7253,8 +7249,8 @@
       <c r="G113" t="s">
         <v>793</v>
       </c>
-      <c r="H113" s="3" t="s">
-        <v>1085</v>
+      <c r="H113" t="s">
+        <v>1084</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
@@ -7279,8 +7275,8 @@
       <c r="G114" t="s">
         <v>794</v>
       </c>
-      <c r="H114" s="3" t="s">
-        <v>1086</v>
+      <c r="H114" t="s">
+        <v>1085</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
@@ -7305,8 +7301,8 @@
       <c r="G115" t="s">
         <v>795</v>
       </c>
-      <c r="H115" s="3" t="s">
-        <v>1087</v>
+      <c r="H115" t="s">
+        <v>1086</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
@@ -7331,8 +7327,8 @@
       <c r="G116" t="s">
         <v>796</v>
       </c>
-      <c r="H116" s="3" t="s">
-        <v>1088</v>
+      <c r="H116" t="s">
+        <v>1087</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
@@ -7357,8 +7353,8 @@
       <c r="G117" t="s">
         <v>797</v>
       </c>
-      <c r="H117" s="3" t="s">
-        <v>1089</v>
+      <c r="H117" t="s">
+        <v>1088</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
@@ -7383,8 +7379,8 @@
       <c r="G118" t="s">
         <v>797</v>
       </c>
-      <c r="H118" s="3" t="s">
-        <v>1090</v>
+      <c r="H118" t="s">
+        <v>1089</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
@@ -7409,8 +7405,8 @@
       <c r="G119" t="s">
         <v>798</v>
       </c>
-      <c r="H119" s="3" t="s">
-        <v>1091</v>
+      <c r="H119" t="s">
+        <v>1090</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
@@ -7435,8 +7431,8 @@
       <c r="G120" t="s">
         <v>796</v>
       </c>
-      <c r="H120" s="3" t="s">
-        <v>1092</v>
+      <c r="H120" t="s">
+        <v>1091</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
@@ -7461,8 +7457,8 @@
       <c r="G121" t="s">
         <v>799</v>
       </c>
-      <c r="H121" s="3" t="s">
-        <v>1093</v>
+      <c r="H121" t="s">
+        <v>1092</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
@@ -7487,8 +7483,8 @@
       <c r="G122" t="s">
         <v>796</v>
       </c>
-      <c r="H122" s="3" t="s">
-        <v>1094</v>
+      <c r="H122" t="s">
+        <v>1093</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
@@ -7513,8 +7509,8 @@
       <c r="G123" t="s">
         <v>800</v>
       </c>
-      <c r="H123" s="3" t="s">
-        <v>1095</v>
+      <c r="H123" t="s">
+        <v>1094</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
@@ -7539,8 +7535,8 @@
       <c r="G124" t="s">
         <v>801</v>
       </c>
-      <c r="H124" s="3" t="s">
-        <v>1096</v>
+      <c r="H124" t="s">
+        <v>1095</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
@@ -7565,8 +7561,8 @@
       <c r="G125" t="s">
         <v>143</v>
       </c>
-      <c r="H125" s="3" t="s">
-        <v>1097</v>
+      <c r="H125" t="s">
+        <v>1096</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
@@ -7591,8 +7587,8 @@
       <c r="G126" t="s">
         <v>803</v>
       </c>
-      <c r="H126" s="3" t="s">
-        <v>1098</v>
+      <c r="H126" t="s">
+        <v>1097</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
@@ -7617,8 +7613,8 @@
       <c r="G127" t="s">
         <v>804</v>
       </c>
-      <c r="H127" s="3" t="s">
-        <v>1099</v>
+      <c r="H127" t="s">
+        <v>1098</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
@@ -7643,8 +7639,8 @@
       <c r="G128" t="s">
         <v>805</v>
       </c>
-      <c r="H128" s="3" t="s">
-        <v>1100</v>
+      <c r="H128" t="s">
+        <v>1099</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
@@ -7669,8 +7665,8 @@
       <c r="G129" t="s">
         <v>969</v>
       </c>
-      <c r="H129" s="3" t="s">
-        <v>1101</v>
+      <c r="H129" t="s">
+        <v>1100</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
@@ -7695,8 +7691,8 @@
       <c r="G130" t="s">
         <v>802</v>
       </c>
-      <c r="H130" s="3" t="s">
-        <v>1102</v>
+      <c r="H130" t="s">
+        <v>1101</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
@@ -7721,8 +7717,8 @@
       <c r="G131" t="s">
         <v>806</v>
       </c>
-      <c r="H131" s="3" t="s">
-        <v>1103</v>
+      <c r="H131" t="s">
+        <v>1102</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
@@ -7747,8 +7743,8 @@
       <c r="G132" t="s">
         <v>807</v>
       </c>
-      <c r="H132" s="3" t="s">
-        <v>1104</v>
+      <c r="H132" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
@@ -7773,8 +7769,8 @@
       <c r="G133" t="s">
         <v>808</v>
       </c>
-      <c r="H133" s="3" t="s">
-        <v>1105</v>
+      <c r="H133" t="s">
+        <v>1104</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
@@ -7799,8 +7795,8 @@
       <c r="G134" t="s">
         <v>809</v>
       </c>
-      <c r="H134" s="3" t="s">
-        <v>1106</v>
+      <c r="H134" t="s">
+        <v>1105</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
@@ -7825,8 +7821,8 @@
       <c r="G135" t="s">
         <v>810</v>
       </c>
-      <c r="H135" s="3" t="s">
-        <v>1107</v>
+      <c r="H135" t="s">
+        <v>1106</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
@@ -7851,8 +7847,8 @@
       <c r="G136" t="s">
         <v>811</v>
       </c>
-      <c r="H136" s="3" t="s">
-        <v>1108</v>
+      <c r="H136" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
@@ -7877,8 +7873,8 @@
       <c r="G137" t="s">
         <v>812</v>
       </c>
-      <c r="H137" s="3" t="s">
-        <v>1109</v>
+      <c r="H137" t="s">
+        <v>1108</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
@@ -7903,8 +7899,8 @@
       <c r="G138" t="s">
         <v>812</v>
       </c>
-      <c r="H138" s="3" t="s">
-        <v>1110</v>
+      <c r="H138" t="s">
+        <v>1109</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
@@ -7929,8 +7925,8 @@
       <c r="G139" t="s">
         <v>153</v>
       </c>
-      <c r="H139" s="3" t="s">
-        <v>1111</v>
+      <c r="H139" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
@@ -7955,8 +7951,8 @@
       <c r="G140" t="s">
         <v>813</v>
       </c>
-      <c r="H140" s="3" t="s">
-        <v>1112</v>
+      <c r="H140" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
@@ -7981,8 +7977,8 @@
       <c r="G141" t="s">
         <v>814</v>
       </c>
-      <c r="H141" s="3" t="s">
-        <v>1113</v>
+      <c r="H141" t="s">
+        <v>1112</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
@@ -8007,8 +8003,8 @@
       <c r="G142" t="s">
         <v>815</v>
       </c>
-      <c r="H142" s="3" t="s">
-        <v>1114</v>
+      <c r="H142" t="s">
+        <v>1113</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
@@ -8033,8 +8029,8 @@
       <c r="G143" t="s">
         <v>812</v>
       </c>
-      <c r="H143" s="3" t="s">
-        <v>1115</v>
+      <c r="H143" t="s">
+        <v>1114</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
@@ -8059,8 +8055,8 @@
       <c r="G144" t="s">
         <v>812</v>
       </c>
-      <c r="H144" s="3" t="s">
-        <v>1116</v>
+      <c r="H144" t="s">
+        <v>1115</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
@@ -8085,8 +8081,8 @@
       <c r="G145" t="s">
         <v>812</v>
       </c>
-      <c r="H145" s="3" t="s">
-        <v>1117</v>
+      <c r="H145" t="s">
+        <v>1116</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
@@ -8111,8 +8107,8 @@
       <c r="G146" t="s">
         <v>816</v>
       </c>
-      <c r="H146" s="3" t="s">
-        <v>1118</v>
+      <c r="H146" t="s">
+        <v>1117</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
@@ -8137,8 +8133,8 @@
       <c r="G147" t="s">
         <v>239</v>
       </c>
-      <c r="H147" s="3" t="s">
-        <v>1119</v>
+      <c r="H147" t="s">
+        <v>1118</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
@@ -8163,8 +8159,8 @@
       <c r="G148" t="s">
         <v>153</v>
       </c>
-      <c r="H148" s="3" t="s">
-        <v>1120</v>
+      <c r="H148" t="s">
+        <v>1119</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
@@ -8189,8 +8185,8 @@
       <c r="G149" t="s">
         <v>815</v>
       </c>
-      <c r="H149" s="3" t="s">
-        <v>1121</v>
+      <c r="H149" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
@@ -8215,8 +8211,8 @@
       <c r="G150" t="s">
         <v>812</v>
       </c>
-      <c r="H150" s="3" t="s">
-        <v>1122</v>
+      <c r="H150" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
@@ -8241,8 +8237,8 @@
       <c r="G151" t="s">
         <v>812</v>
       </c>
-      <c r="H151" s="3" t="s">
-        <v>1123</v>
+      <c r="H151" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
@@ -8267,8 +8263,8 @@
       <c r="G152" t="s">
         <v>168</v>
       </c>
-      <c r="H152" s="3" t="s">
-        <v>1124</v>
+      <c r="H152" t="s">
+        <v>1123</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
@@ -8293,8 +8289,8 @@
       <c r="G153" t="s">
         <v>817</v>
       </c>
-      <c r="H153" s="3" t="s">
-        <v>1125</v>
+      <c r="H153" t="s">
+        <v>1124</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
@@ -8319,8 +8315,8 @@
       <c r="G154" t="s">
         <v>799</v>
       </c>
-      <c r="H154" s="3" t="s">
-        <v>1126</v>
+      <c r="H154" t="s">
+        <v>1125</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
@@ -8345,8 +8341,8 @@
       <c r="G155" t="s">
         <v>7</v>
       </c>
-      <c r="H155" s="3" t="s">
-        <v>1127</v>
+      <c r="H155" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
@@ -8371,8 +8367,8 @@
       <c r="G156" t="s">
         <v>818</v>
       </c>
-      <c r="H156" s="3" t="s">
-        <v>1128</v>
+      <c r="H156" t="s">
+        <v>1127</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
@@ -8397,8 +8393,8 @@
       <c r="G157" t="s">
         <v>819</v>
       </c>
-      <c r="H157" s="3" t="s">
-        <v>1129</v>
+      <c r="H157" t="s">
+        <v>1128</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
@@ -8423,8 +8419,8 @@
       <c r="G158" t="s">
         <v>820</v>
       </c>
-      <c r="H158" s="3" t="s">
-        <v>1130</v>
+      <c r="H158" t="s">
+        <v>1129</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
@@ -8449,8 +8445,8 @@
       <c r="G159" t="s">
         <v>791</v>
       </c>
-      <c r="H159" s="3" t="s">
-        <v>1131</v>
+      <c r="H159" t="s">
+        <v>1130</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
@@ -8470,13 +8466,13 @@
         <v>416</v>
       </c>
       <c r="F160" t="s">
+        <v>971</v>
+      </c>
+      <c r="G160" t="s">
         <v>972</v>
       </c>
-      <c r="G160" t="s">
-        <v>973</v>
-      </c>
-      <c r="H160" s="3" t="s">
-        <v>1132</v>
+      <c r="H160" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
@@ -8501,8 +8497,8 @@
       <c r="G161" t="s">
         <v>820</v>
       </c>
-      <c r="H161" s="3" t="s">
-        <v>1133</v>
+      <c r="H161" t="s">
+        <v>1132</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.3">
@@ -8527,8 +8523,8 @@
       <c r="G162" t="s">
         <v>821</v>
       </c>
-      <c r="H162" s="3" t="s">
-        <v>1134</v>
+      <c r="H162" t="s">
+        <v>1133</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
@@ -8553,8 +8549,8 @@
       <c r="G163" t="s">
         <v>822</v>
       </c>
-      <c r="H163" s="3" t="s">
-        <v>1135</v>
+      <c r="H163" t="s">
+        <v>1134</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
@@ -8579,8 +8575,8 @@
       <c r="G164" t="s">
         <v>823</v>
       </c>
-      <c r="H164" s="3" t="s">
-        <v>1136</v>
+      <c r="H164" t="s">
+        <v>1135</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
@@ -8605,8 +8601,8 @@
       <c r="G165" t="s">
         <v>97</v>
       </c>
-      <c r="H165" s="3" t="s">
-        <v>1137</v>
+      <c r="H165" t="s">
+        <v>1136</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
@@ -8631,8 +8627,8 @@
       <c r="G166" t="s">
         <v>771</v>
       </c>
-      <c r="H166" s="3" t="s">
-        <v>1138</v>
+      <c r="H166" t="s">
+        <v>1137</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
@@ -8657,8 +8653,8 @@
       <c r="G167" t="s">
         <v>824</v>
       </c>
-      <c r="H167" s="3" t="s">
-        <v>1139</v>
+      <c r="H167" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
@@ -8683,8 +8679,8 @@
       <c r="G168" t="s">
         <v>825</v>
       </c>
-      <c r="H168" s="3" t="s">
-        <v>1140</v>
+      <c r="H168" t="s">
+        <v>1139</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
@@ -8709,8 +8705,8 @@
       <c r="G169" t="s">
         <v>188</v>
       </c>
-      <c r="H169" s="3" t="s">
-        <v>1141</v>
+      <c r="H169" t="s">
+        <v>1140</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
@@ -8735,8 +8731,8 @@
       <c r="G170" t="s">
         <v>826</v>
       </c>
-      <c r="H170" s="3" t="s">
-        <v>1142</v>
+      <c r="H170" t="s">
+        <v>1141</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
@@ -8761,8 +8757,8 @@
       <c r="G171" t="s">
         <v>827</v>
       </c>
-      <c r="H171" s="3" t="s">
-        <v>1143</v>
+      <c r="H171" t="s">
+        <v>1142</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
@@ -8787,8 +8783,8 @@
       <c r="G172" t="s">
         <v>192</v>
       </c>
-      <c r="H172" s="3" t="s">
-        <v>1144</v>
+      <c r="H172" t="s">
+        <v>1143</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.3">
@@ -8813,8 +8809,8 @@
       <c r="G173" t="s">
         <v>808</v>
       </c>
-      <c r="H173" s="3" t="s">
-        <v>1145</v>
+      <c r="H173" t="s">
+        <v>1144</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.3">
@@ -8839,8 +8835,8 @@
       <c r="G174" t="s">
         <v>828</v>
       </c>
-      <c r="H174" s="3" t="s">
-        <v>1146</v>
+      <c r="H174" t="s">
+        <v>1145</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
@@ -8865,8 +8861,8 @@
       <c r="G175" t="s">
         <v>968</v>
       </c>
-      <c r="H175" s="3" t="s">
-        <v>1147</v>
+      <c r="H175" t="s">
+        <v>1146</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.3">
@@ -8891,8 +8887,8 @@
       <c r="G176" t="s">
         <v>829</v>
       </c>
-      <c r="H176" s="3" t="s">
-        <v>1148</v>
+      <c r="H176" t="s">
+        <v>1147</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.3">
@@ -8917,8 +8913,8 @@
       <c r="G177" t="s">
         <v>830</v>
       </c>
-      <c r="H177" s="3" t="s">
-        <v>1149</v>
+      <c r="H177" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
@@ -8943,8 +8939,8 @@
       <c r="G178" t="s">
         <v>831</v>
       </c>
-      <c r="H178" s="3" t="s">
-        <v>1150</v>
+      <c r="H178" t="s">
+        <v>1149</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
@@ -8969,8 +8965,8 @@
       <c r="G179" t="s">
         <v>832</v>
       </c>
-      <c r="H179" s="3" t="s">
-        <v>1151</v>
+      <c r="H179" t="s">
+        <v>1150</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
@@ -8995,8 +8991,8 @@
       <c r="G180" t="s">
         <v>833</v>
       </c>
-      <c r="H180" s="3" t="s">
-        <v>1152</v>
+      <c r="H180" t="s">
+        <v>1151</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.3">
@@ -9021,8 +9017,8 @@
       <c r="G181" t="s">
         <v>834</v>
       </c>
-      <c r="H181" s="3" t="s">
-        <v>1153</v>
+      <c r="H181" t="s">
+        <v>1152</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.3">
@@ -9047,8 +9043,8 @@
       <c r="G182" t="s">
         <v>835</v>
       </c>
-      <c r="H182" s="3" t="s">
-        <v>1154</v>
+      <c r="H182" t="s">
+        <v>1153</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
@@ -9073,8 +9069,8 @@
       <c r="G183" t="s">
         <v>211</v>
       </c>
-      <c r="H183" s="3" t="s">
-        <v>1155</v>
+      <c r="H183" t="s">
+        <v>1154</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
@@ -9099,8 +9095,8 @@
       <c r="G184" t="s">
         <v>836</v>
       </c>
-      <c r="H184" s="3" t="s">
-        <v>1156</v>
+      <c r="H184" t="s">
+        <v>1155</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
@@ -9125,8 +9121,8 @@
       <c r="G185" t="s">
         <v>837</v>
       </c>
-      <c r="H185" s="3" t="s">
-        <v>1157</v>
+      <c r="H185" t="s">
+        <v>1156</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
@@ -9151,8 +9147,8 @@
       <c r="G186" t="s">
         <v>838</v>
       </c>
-      <c r="H186" s="3" t="s">
-        <v>1158</v>
+      <c r="H186" t="s">
+        <v>1157</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
@@ -9177,8 +9173,8 @@
       <c r="G187" t="s">
         <v>839</v>
       </c>
-      <c r="H187" s="3" t="s">
-        <v>1159</v>
+      <c r="H187" t="s">
+        <v>1158</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -9203,8 +9199,8 @@
       <c r="G188" t="s">
         <v>839</v>
       </c>
-      <c r="H188" s="3" t="s">
-        <v>1160</v>
+      <c r="H188" t="s">
+        <v>1159</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.3">
@@ -9229,8 +9225,8 @@
       <c r="G189" t="s">
         <v>840</v>
       </c>
-      <c r="H189" s="3" t="s">
-        <v>1161</v>
+      <c r="H189" t="s">
+        <v>1160</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
@@ -9255,8 +9251,8 @@
       <c r="G190" t="s">
         <v>839</v>
       </c>
-      <c r="H190" s="3" t="s">
-        <v>1162</v>
+      <c r="H190" t="s">
+        <v>1161</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
@@ -9281,8 +9277,8 @@
       <c r="G191" t="s">
         <v>841</v>
       </c>
-      <c r="H191" s="3" t="s">
-        <v>1163</v>
+      <c r="H191" t="s">
+        <v>1162</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
@@ -9307,8 +9303,8 @@
       <c r="G192" t="s">
         <v>842</v>
       </c>
-      <c r="H192" s="3" t="s">
-        <v>1164</v>
+      <c r="H192" t="s">
+        <v>1163</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.3">
@@ -9333,8 +9329,8 @@
       <c r="G193" t="s">
         <v>843</v>
       </c>
-      <c r="H193" s="3" t="s">
-        <v>1165</v>
+      <c r="H193" t="s">
+        <v>1164</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
@@ -9359,8 +9355,8 @@
       <c r="G194" t="s">
         <v>844</v>
       </c>
-      <c r="H194" s="3" t="s">
-        <v>1166</v>
+      <c r="H194" t="s">
+        <v>1165</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
@@ -9385,8 +9381,8 @@
       <c r="G195" t="s">
         <v>845</v>
       </c>
-      <c r="H195" s="3" t="s">
-        <v>1167</v>
+      <c r="H195" t="s">
+        <v>1166</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
@@ -9411,8 +9407,8 @@
       <c r="G196" t="s">
         <v>846</v>
       </c>
-      <c r="H196" s="3" t="s">
-        <v>1168</v>
+      <c r="H196" t="s">
+        <v>1167</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.3">
@@ -9437,8 +9433,8 @@
       <c r="G197" t="s">
         <v>847</v>
       </c>
-      <c r="H197" s="3" t="s">
-        <v>1169</v>
+      <c r="H197" t="s">
+        <v>1168</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.3">
@@ -9463,8 +9459,8 @@
       <c r="G198" t="s">
         <v>846</v>
       </c>
-      <c r="H198" s="3" t="s">
-        <v>1170</v>
+      <c r="H198" t="s">
+        <v>1169</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
@@ -9489,8 +9485,8 @@
       <c r="G199" t="s">
         <v>846</v>
       </c>
-      <c r="H199" s="3" t="s">
-        <v>1171</v>
+      <c r="H199" t="s">
+        <v>1170</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
@@ -9515,8 +9511,8 @@
       <c r="G200" t="s">
         <v>846</v>
       </c>
-      <c r="H200" s="3" t="s">
-        <v>1172</v>
+      <c r="H200" t="s">
+        <v>1171</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
@@ -9541,8 +9537,8 @@
       <c r="G201" t="s">
         <v>846</v>
       </c>
-      <c r="H201" s="3" t="s">
-        <v>1173</v>
+      <c r="H201" t="s">
+        <v>1172</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
@@ -9567,8 +9563,8 @@
       <c r="G202" t="s">
         <v>224</v>
       </c>
-      <c r="H202" s="3" t="s">
-        <v>1174</v>
+      <c r="H202" t="s">
+        <v>1173</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
@@ -9593,8 +9589,8 @@
       <c r="G203" t="s">
         <v>846</v>
       </c>
-      <c r="H203" s="3" t="s">
-        <v>1175</v>
+      <c r="H203" t="s">
+        <v>1174</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
@@ -9619,8 +9615,8 @@
       <c r="G204" t="s">
         <v>848</v>
       </c>
-      <c r="H204" s="3" t="s">
-        <v>1176</v>
+      <c r="H204" t="s">
+        <v>1175</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.3">
@@ -9645,8 +9641,8 @@
       <c r="G205" t="s">
         <v>849</v>
       </c>
-      <c r="H205" s="3" t="s">
-        <v>1177</v>
+      <c r="H205" t="s">
+        <v>1176</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
@@ -9671,8 +9667,8 @@
       <c r="G206" t="s">
         <v>227</v>
       </c>
-      <c r="H206" s="3" t="s">
-        <v>1178</v>
+      <c r="H206" t="s">
+        <v>1177</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
@@ -9697,8 +9693,8 @@
       <c r="G207" t="s">
         <v>850</v>
       </c>
-      <c r="H207" s="3" t="s">
-        <v>1179</v>
+      <c r="H207" t="s">
+        <v>1178</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
@@ -9723,8 +9719,8 @@
       <c r="G208" t="s">
         <v>851</v>
       </c>
-      <c r="H208" s="3" t="s">
-        <v>1180</v>
+      <c r="H208" t="s">
+        <v>1179</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
@@ -9747,10 +9743,10 @@
         <v>965</v>
       </c>
       <c r="G209" t="s">
-        <v>1287</v>
-      </c>
-      <c r="H209" s="3" t="s">
-        <v>1289</v>
+        <v>1286</v>
+      </c>
+      <c r="H209" t="s">
+        <v>1288</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
@@ -9775,8 +9771,8 @@
       <c r="G210" t="s">
         <v>852</v>
       </c>
-      <c r="H210" s="3" t="s">
-        <v>1181</v>
+      <c r="H210" t="s">
+        <v>1180</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
@@ -9801,8 +9797,8 @@
       <c r="G211" t="s">
         <v>853</v>
       </c>
-      <c r="H211" s="3" t="s">
-        <v>1182</v>
+      <c r="H211" t="s">
+        <v>1181</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
@@ -9825,10 +9821,10 @@
         <v>646</v>
       </c>
       <c r="G212" t="s">
-        <v>1288</v>
-      </c>
-      <c r="H212" s="3" t="s">
-        <v>1290</v>
+        <v>1287</v>
+      </c>
+      <c r="H212" t="s">
+        <v>1289</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
@@ -9853,8 +9849,8 @@
       <c r="G213" t="s">
         <v>855</v>
       </c>
-      <c r="H213" s="3" t="s">
-        <v>1183</v>
+      <c r="H213" t="s">
+        <v>1182</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
@@ -9879,8 +9875,8 @@
       <c r="G214" t="s">
         <v>854</v>
       </c>
-      <c r="H214" s="3" t="s">
-        <v>1184</v>
+      <c r="H214" t="s">
+        <v>1183</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
@@ -9905,8 +9901,8 @@
       <c r="G215" t="s">
         <v>855</v>
       </c>
-      <c r="H215" s="3" t="s">
-        <v>1185</v>
+      <c r="H215" t="s">
+        <v>1184</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.3">
@@ -9931,8 +9927,8 @@
       <c r="G216" t="s">
         <v>855</v>
       </c>
-      <c r="H216" s="3" t="s">
-        <v>1186</v>
+      <c r="H216" t="s">
+        <v>1185</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.3">
@@ -9957,8 +9953,8 @@
       <c r="G217" t="s">
         <v>851</v>
       </c>
-      <c r="H217" s="3" t="s">
-        <v>1187</v>
+      <c r="H217" t="s">
+        <v>1186</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
@@ -9983,8 +9979,8 @@
       <c r="G218" t="s">
         <v>855</v>
       </c>
-      <c r="H218" s="3" t="s">
-        <v>1188</v>
+      <c r="H218" t="s">
+        <v>1187</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
@@ -10009,8 +10005,8 @@
       <c r="G219" t="s">
         <v>856</v>
       </c>
-      <c r="H219" s="3" t="s">
-        <v>1189</v>
+      <c r="H219" t="s">
+        <v>1188</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.3">
@@ -10035,8 +10031,8 @@
       <c r="G220" t="s">
         <v>857</v>
       </c>
-      <c r="H220" s="3" t="s">
-        <v>1190</v>
+      <c r="H220" t="s">
+        <v>1189</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.3">
@@ -10061,8 +10057,8 @@
       <c r="G221" t="s">
         <v>858</v>
       </c>
-      <c r="H221" s="3" t="s">
-        <v>1191</v>
+      <c r="H221" t="s">
+        <v>1190</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.3">
@@ -10087,8 +10083,8 @@
       <c r="G222" t="s">
         <v>859</v>
       </c>
-      <c r="H222" s="3" t="s">
-        <v>1192</v>
+      <c r="H222" t="s">
+        <v>1191</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
@@ -10113,8 +10109,8 @@
       <c r="G223" t="s">
         <v>860</v>
       </c>
-      <c r="H223" s="3" t="s">
-        <v>1193</v>
+      <c r="H223" t="s">
+        <v>1192</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
@@ -10139,8 +10135,8 @@
       <c r="G224" t="s">
         <v>791</v>
       </c>
-      <c r="H224" s="3" t="s">
-        <v>1194</v>
+      <c r="H224" t="s">
+        <v>1193</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
@@ -10165,8 +10161,8 @@
       <c r="G225" t="s">
         <v>861</v>
       </c>
-      <c r="H225" s="3" t="s">
-        <v>1195</v>
+      <c r="H225" t="s">
+        <v>1194</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
@@ -10191,8 +10187,8 @@
       <c r="G226" t="s">
         <v>743</v>
       </c>
-      <c r="H226" s="3" t="s">
-        <v>1196</v>
+      <c r="H226" t="s">
+        <v>1195</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.3">
@@ -10217,8 +10213,8 @@
       <c r="G227" t="s">
         <v>958</v>
       </c>
-      <c r="H227" s="3" t="s">
-        <v>1197</v>
+      <c r="H227" t="s">
+        <v>1196</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
@@ -10243,8 +10239,8 @@
       <c r="G228" t="s">
         <v>861</v>
       </c>
-      <c r="H228" s="3" t="s">
-        <v>1198</v>
+      <c r="H228" t="s">
+        <v>1197</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.3">
@@ -10269,8 +10265,8 @@
       <c r="G229" t="s">
         <v>211</v>
       </c>
-      <c r="H229" s="3" t="s">
-        <v>1199</v>
+      <c r="H229" t="s">
+        <v>1198</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.3">
@@ -10295,8 +10291,8 @@
       <c r="G230" t="s">
         <v>862</v>
       </c>
-      <c r="H230" s="3" t="s">
-        <v>1200</v>
+      <c r="H230" t="s">
+        <v>1199</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.3">
@@ -10321,8 +10317,8 @@
       <c r="G231" t="s">
         <v>912</v>
       </c>
-      <c r="H231" s="3" t="s">
-        <v>1201</v>
+      <c r="H231" t="s">
+        <v>1200</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.3">
@@ -10347,8 +10343,8 @@
       <c r="G232" t="s">
         <v>863</v>
       </c>
-      <c r="H232" s="3" t="s">
-        <v>1202</v>
+      <c r="H232" t="s">
+        <v>1201</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.3">
@@ -10373,8 +10369,8 @@
       <c r="G233" t="s">
         <v>864</v>
       </c>
-      <c r="H233" s="3" t="s">
-        <v>1203</v>
+      <c r="H233" t="s">
+        <v>1202</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.3">
@@ -10399,8 +10395,8 @@
       <c r="G234" t="s">
         <v>865</v>
       </c>
-      <c r="H234" s="3" t="s">
-        <v>1204</v>
+      <c r="H234" t="s">
+        <v>1203</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.3">
@@ -10425,8 +10421,8 @@
       <c r="G235" t="s">
         <v>960</v>
       </c>
-      <c r="H235" s="3" t="s">
-        <v>1205</v>
+      <c r="H235" t="s">
+        <v>1204</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.3">
@@ -10451,8 +10447,8 @@
       <c r="G236" t="s">
         <v>866</v>
       </c>
-      <c r="H236" s="3" t="s">
-        <v>1206</v>
+      <c r="H236" t="s">
+        <v>1205</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.3">
@@ -10477,8 +10473,8 @@
       <c r="G237" t="s">
         <v>757</v>
       </c>
-      <c r="H237" s="3" t="s">
-        <v>1207</v>
+      <c r="H237" t="s">
+        <v>1206</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.3">
@@ -10503,8 +10499,8 @@
       <c r="G238" t="s">
         <v>867</v>
       </c>
-      <c r="H238" s="3" t="s">
-        <v>1208</v>
+      <c r="H238" t="s">
+        <v>1207</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.3">
@@ -10529,8 +10525,8 @@
       <c r="G239" t="s">
         <v>764</v>
       </c>
-      <c r="H239" s="3" t="s">
-        <v>1209</v>
+      <c r="H239" t="s">
+        <v>1208</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.3">
@@ -10555,8 +10551,8 @@
       <c r="G240" t="s">
         <v>261</v>
       </c>
-      <c r="H240" s="3" t="s">
-        <v>1210</v>
+      <c r="H240" t="s">
+        <v>1209</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.3">
@@ -10581,8 +10577,8 @@
       <c r="G241" t="s">
         <v>868</v>
       </c>
-      <c r="H241" s="3" t="s">
-        <v>1211</v>
+      <c r="H241" t="s">
+        <v>1210</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.3">
@@ -10607,8 +10603,8 @@
       <c r="G242" t="s">
         <v>869</v>
       </c>
-      <c r="H242" s="3" t="s">
-        <v>1212</v>
+      <c r="H242" t="s">
+        <v>1211</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.3">
@@ -10633,8 +10629,8 @@
       <c r="G243" t="s">
         <v>870</v>
       </c>
-      <c r="H243" s="3" t="s">
-        <v>1213</v>
+      <c r="H243" t="s">
+        <v>1212</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.3">
@@ -10659,8 +10655,8 @@
       <c r="G244" t="s">
         <v>871</v>
       </c>
-      <c r="H244" s="3" t="s">
-        <v>1214</v>
+      <c r="H244" t="s">
+        <v>1213</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.3">
@@ -10685,8 +10681,8 @@
       <c r="G245" t="s">
         <v>872</v>
       </c>
-      <c r="H245" s="3" t="s">
-        <v>1215</v>
+      <c r="H245" t="s">
+        <v>1214</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.3">
@@ -10711,8 +10707,8 @@
       <c r="G246" t="s">
         <v>873</v>
       </c>
-      <c r="H246" s="3" t="s">
-        <v>1216</v>
+      <c r="H246" t="s">
+        <v>1215</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.3">
@@ -10737,8 +10733,8 @@
       <c r="G247" t="s">
         <v>874</v>
       </c>
-      <c r="H247" s="3" t="s">
-        <v>1217</v>
+      <c r="H247" t="s">
+        <v>1216</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.3">
@@ -10763,8 +10759,8 @@
       <c r="G248" t="s">
         <v>875</v>
       </c>
-      <c r="H248" s="3" t="s">
-        <v>1218</v>
+      <c r="H248" t="s">
+        <v>1217</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.3">
@@ -10789,8 +10785,8 @@
       <c r="G249" t="s">
         <v>876</v>
       </c>
-      <c r="H249" s="3" t="s">
-        <v>1219</v>
+      <c r="H249" t="s">
+        <v>1218</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.3">
@@ -10815,8 +10811,8 @@
       <c r="G250" t="s">
         <v>274</v>
       </c>
-      <c r="H250" s="3" t="s">
-        <v>1220</v>
+      <c r="H250" t="s">
+        <v>1219</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.3">
@@ -10841,8 +10837,8 @@
       <c r="G251" t="s">
         <v>877</v>
       </c>
-      <c r="H251" s="3" t="s">
-        <v>1221</v>
+      <c r="H251" t="s">
+        <v>1220</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.3">
@@ -10867,8 +10863,8 @@
       <c r="G252" t="s">
         <v>877</v>
       </c>
-      <c r="H252" s="3" t="s">
-        <v>1222</v>
+      <c r="H252" t="s">
+        <v>1221</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.3">
@@ -10893,8 +10889,8 @@
       <c r="G253" t="s">
         <v>878</v>
       </c>
-      <c r="H253" s="3" t="s">
-        <v>1223</v>
+      <c r="H253" t="s">
+        <v>1222</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.3">
@@ -10919,8 +10915,8 @@
       <c r="G254" t="s">
         <v>879</v>
       </c>
-      <c r="H254" s="3" t="s">
-        <v>1224</v>
+      <c r="H254" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.3">
@@ -10945,8 +10941,8 @@
       <c r="G255" t="s">
         <v>880</v>
       </c>
-      <c r="H255" s="3" t="s">
-        <v>1225</v>
+      <c r="H255" t="s">
+        <v>1224</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.3">
@@ -10971,8 +10967,8 @@
       <c r="G256" t="s">
         <v>881</v>
       </c>
-      <c r="H256" s="3" t="s">
-        <v>1226</v>
+      <c r="H256" t="s">
+        <v>1225</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.3">
@@ -10997,8 +10993,8 @@
       <c r="G257" t="s">
         <v>274</v>
       </c>
-      <c r="H257" s="3" t="s">
-        <v>1227</v>
+      <c r="H257" t="s">
+        <v>1226</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.3">
@@ -11023,8 +11019,8 @@
       <c r="G258" t="s">
         <v>877</v>
       </c>
-      <c r="H258" s="3" t="s">
-        <v>1228</v>
+      <c r="H258" t="s">
+        <v>1227</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.3">
@@ -11049,8 +11045,8 @@
       <c r="G259" t="s">
         <v>882</v>
       </c>
-      <c r="H259" s="3" t="s">
-        <v>1229</v>
+      <c r="H259" t="s">
+        <v>1228</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.3">
@@ -11075,8 +11071,8 @@
       <c r="G260" t="s">
         <v>883</v>
       </c>
-      <c r="H260" s="3" t="s">
-        <v>1230</v>
+      <c r="H260" t="s">
+        <v>1229</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.3">
@@ -11101,8 +11097,8 @@
       <c r="G261" t="s">
         <v>884</v>
       </c>
-      <c r="H261" s="3" t="s">
-        <v>1231</v>
+      <c r="H261" t="s">
+        <v>1230</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.3">
@@ -11127,8 +11123,8 @@
       <c r="G262" t="s">
         <v>883</v>
       </c>
-      <c r="H262" s="3" t="s">
-        <v>1232</v>
+      <c r="H262" t="s">
+        <v>1231</v>
       </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.3">
@@ -11153,8 +11149,8 @@
       <c r="G263" t="s">
         <v>798</v>
       </c>
-      <c r="H263" s="3" t="s">
-        <v>1233</v>
+      <c r="H263" t="s">
+        <v>1232</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.3">
@@ -11179,8 +11175,8 @@
       <c r="G264" t="s">
         <v>295</v>
       </c>
-      <c r="H264" s="3" t="s">
-        <v>1234</v>
+      <c r="H264" t="s">
+        <v>1233</v>
       </c>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.3">
@@ -11205,8 +11201,8 @@
       <c r="G265" t="s">
         <v>885</v>
       </c>
-      <c r="H265" s="3" t="s">
-        <v>1235</v>
+      <c r="H265" t="s">
+        <v>1234</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.3">
@@ -11231,8 +11227,8 @@
       <c r="G266" t="s">
         <v>859</v>
       </c>
-      <c r="H266" s="3" t="s">
-        <v>1236</v>
+      <c r="H266" t="s">
+        <v>1235</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.3">
@@ -11257,8 +11253,8 @@
       <c r="G267" t="s">
         <v>886</v>
       </c>
-      <c r="H267" s="3" t="s">
-        <v>1237</v>
+      <c r="H267" t="s">
+        <v>1236</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.3">
@@ -11283,8 +11279,8 @@
       <c r="G268" t="s">
         <v>295</v>
       </c>
-      <c r="H268" s="3" t="s">
-        <v>1238</v>
+      <c r="H268" t="s">
+        <v>1237</v>
       </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.3">
@@ -11309,8 +11305,8 @@
       <c r="G269" t="s">
         <v>887</v>
       </c>
-      <c r="H269" s="3" t="s">
-        <v>1239</v>
+      <c r="H269" t="s">
+        <v>1238</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.3">
@@ -11335,8 +11331,8 @@
       <c r="G270" t="s">
         <v>883</v>
       </c>
-      <c r="H270" s="3" t="s">
-        <v>1240</v>
+      <c r="H270" t="s">
+        <v>1239</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.3">
@@ -11361,8 +11357,8 @@
       <c r="G271" t="s">
         <v>798</v>
       </c>
-      <c r="H271" s="3" t="s">
-        <v>1241</v>
+      <c r="H271" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.3">
@@ -11387,8 +11383,8 @@
       <c r="G272" t="s">
         <v>295</v>
       </c>
-      <c r="H272" s="3" t="s">
-        <v>1242</v>
+      <c r="H272" t="s">
+        <v>1241</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.3">
@@ -11413,8 +11409,8 @@
       <c r="G273" t="s">
         <v>883</v>
       </c>
-      <c r="H273" s="3" t="s">
-        <v>1243</v>
+      <c r="H273" t="s">
+        <v>1242</v>
       </c>
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.3">
@@ -11439,8 +11435,8 @@
       <c r="G274" t="s">
         <v>295</v>
       </c>
-      <c r="H274" s="3" t="s">
-        <v>1244</v>
+      <c r="H274" t="s">
+        <v>1243</v>
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.3">
@@ -11465,8 +11461,8 @@
       <c r="G275" t="s">
         <v>887</v>
       </c>
-      <c r="H275" s="3" t="s">
-        <v>1245</v>
+      <c r="H275" t="s">
+        <v>1244</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.3">
@@ -11491,8 +11487,8 @@
       <c r="G276" t="s">
         <v>883</v>
       </c>
-      <c r="H276" s="3" t="s">
-        <v>1246</v>
+      <c r="H276" t="s">
+        <v>1245</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.3">
@@ -11517,8 +11513,8 @@
       <c r="G277" t="s">
         <v>883</v>
       </c>
-      <c r="H277" s="3" t="s">
-        <v>1247</v>
+      <c r="H277" t="s">
+        <v>1246</v>
       </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.3">
@@ -11543,8 +11539,8 @@
       <c r="G278" t="s">
         <v>883</v>
       </c>
-      <c r="H278" s="3" t="s">
-        <v>1248</v>
+      <c r="H278" t="s">
+        <v>1247</v>
       </c>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.3">
@@ -11569,8 +11565,8 @@
       <c r="G279" t="s">
         <v>243</v>
       </c>
-      <c r="H279" s="3" t="s">
-        <v>1249</v>
+      <c r="H279" t="s">
+        <v>1248</v>
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.3">
@@ -11595,8 +11591,8 @@
       <c r="G280" t="s">
         <v>962</v>
       </c>
-      <c r="H280" s="3" t="s">
-        <v>1250</v>
+      <c r="H280" t="s">
+        <v>1249</v>
       </c>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.3">
@@ -11621,8 +11617,8 @@
       <c r="G281" t="s">
         <v>888</v>
       </c>
-      <c r="H281" s="3" t="s">
-        <v>1251</v>
+      <c r="H281" t="s">
+        <v>1250</v>
       </c>
     </row>
     <row r="282" spans="1:8" x14ac:dyDescent="0.3">
@@ -11647,8 +11643,8 @@
       <c r="G282" t="s">
         <v>889</v>
       </c>
-      <c r="H282" s="3" t="s">
-        <v>1252</v>
+      <c r="H282" t="s">
+        <v>1251</v>
       </c>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.3">
@@ -11673,8 +11669,8 @@
       <c r="G283" t="s">
         <v>890</v>
       </c>
-      <c r="H283" s="3" t="s">
-        <v>1253</v>
+      <c r="H283" t="s">
+        <v>1252</v>
       </c>
     </row>
     <row r="284" spans="1:8" x14ac:dyDescent="0.3">
@@ -11699,8 +11695,8 @@
       <c r="G284" t="s">
         <v>891</v>
       </c>
-      <c r="H284" s="3" t="s">
-        <v>1254</v>
+      <c r="H284" t="s">
+        <v>1253</v>
       </c>
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.3">
@@ -11725,8 +11721,8 @@
       <c r="G285" t="s">
         <v>892</v>
       </c>
-      <c r="H285" s="3" t="s">
-        <v>1255</v>
+      <c r="H285" t="s">
+        <v>1254</v>
       </c>
     </row>
     <row r="286" spans="1:8" x14ac:dyDescent="0.3">
@@ -11751,8 +11747,8 @@
       <c r="G286" t="s">
         <v>893</v>
       </c>
-      <c r="H286" s="3" t="s">
-        <v>1256</v>
+      <c r="H286" t="s">
+        <v>1255</v>
       </c>
     </row>
     <row r="287" spans="1:8" x14ac:dyDescent="0.3">
@@ -11777,8 +11773,8 @@
       <c r="G287" t="s">
         <v>894</v>
       </c>
-      <c r="H287" s="3" t="s">
-        <v>1257</v>
+      <c r="H287" t="s">
+        <v>1256</v>
       </c>
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.3">
@@ -11803,8 +11799,8 @@
       <c r="G288" t="s">
         <v>894</v>
       </c>
-      <c r="H288" s="3" t="s">
-        <v>1258</v>
+      <c r="H288" t="s">
+        <v>1257</v>
       </c>
     </row>
     <row r="289" spans="1:8" x14ac:dyDescent="0.3">
@@ -11829,8 +11825,8 @@
       <c r="G289" t="s">
         <v>895</v>
       </c>
-      <c r="H289" s="3" t="s">
-        <v>1259</v>
+      <c r="H289" t="s">
+        <v>1258</v>
       </c>
     </row>
     <row r="290" spans="1:8" x14ac:dyDescent="0.3">
@@ -11855,8 +11851,8 @@
       <c r="G290" t="s">
         <v>896</v>
       </c>
-      <c r="H290" s="3" t="s">
-        <v>1260</v>
+      <c r="H290" t="s">
+        <v>1259</v>
       </c>
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.3">
@@ -11881,8 +11877,8 @@
       <c r="G291" t="s">
         <v>311</v>
       </c>
-      <c r="H291" s="3" t="s">
-        <v>1261</v>
+      <c r="H291" t="s">
+        <v>1260</v>
       </c>
     </row>
     <row r="292" spans="1:8" x14ac:dyDescent="0.3">
@@ -11907,8 +11903,8 @@
       <c r="G292" t="s">
         <v>897</v>
       </c>
-      <c r="H292" s="3" t="s">
-        <v>1262</v>
+      <c r="H292" t="s">
+        <v>1261</v>
       </c>
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.3">
@@ -11933,8 +11929,8 @@
       <c r="G293" t="s">
         <v>894</v>
       </c>
-      <c r="H293" s="3" t="s">
-        <v>1263</v>
+      <c r="H293" t="s">
+        <v>1262</v>
       </c>
     </row>
     <row r="294" spans="1:8" x14ac:dyDescent="0.3">
@@ -11959,8 +11955,8 @@
       <c r="G294" t="s">
         <v>312</v>
       </c>
-      <c r="H294" s="3" t="s">
-        <v>1264</v>
+      <c r="H294" t="s">
+        <v>1263</v>
       </c>
     </row>
     <row r="295" spans="1:8" x14ac:dyDescent="0.3">
@@ -11985,8 +11981,8 @@
       <c r="G295" t="s">
         <v>898</v>
       </c>
-      <c r="H295" s="3" t="s">
-        <v>1265</v>
+      <c r="H295" t="s">
+        <v>1264</v>
       </c>
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.3">
@@ -12011,8 +12007,8 @@
       <c r="G296" t="s">
         <v>898</v>
       </c>
-      <c r="H296" s="3" t="s">
-        <v>1266</v>
+      <c r="H296" t="s">
+        <v>1265</v>
       </c>
     </row>
     <row r="297" spans="1:8" x14ac:dyDescent="0.3">
@@ -12037,8 +12033,8 @@
       <c r="G297" t="s">
         <v>899</v>
       </c>
-      <c r="H297" s="3" t="s">
-        <v>1267</v>
+      <c r="H297" t="s">
+        <v>1266</v>
       </c>
     </row>
     <row r="298" spans="1:8" x14ac:dyDescent="0.3">
@@ -12063,8 +12059,8 @@
       <c r="G298" t="s">
         <v>900</v>
       </c>
-      <c r="H298" s="3" t="s">
-        <v>1268</v>
+      <c r="H298" t="s">
+        <v>1267</v>
       </c>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.3">
@@ -12089,8 +12085,8 @@
       <c r="G299" t="s">
         <v>898</v>
       </c>
-      <c r="H299" s="3" t="s">
-        <v>1269</v>
+      <c r="H299" t="s">
+        <v>1268</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.3">
@@ -12115,8 +12111,8 @@
       <c r="G300" t="s">
         <v>901</v>
       </c>
-      <c r="H300" s="3" t="s">
-        <v>1270</v>
+      <c r="H300" t="s">
+        <v>1269</v>
       </c>
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.3">
@@ -12141,8 +12137,8 @@
       <c r="G301" t="s">
         <v>902</v>
       </c>
-      <c r="H301" s="3" t="s">
-        <v>1271</v>
+      <c r="H301" t="s">
+        <v>1270</v>
       </c>
     </row>
     <row r="302" spans="1:8" x14ac:dyDescent="0.3">
@@ -12167,8 +12163,8 @@
       <c r="G302" t="s">
         <v>851</v>
       </c>
-      <c r="H302" s="3" t="s">
-        <v>1272</v>
+      <c r="H302" t="s">
+        <v>1271</v>
       </c>
     </row>
     <row r="303" spans="1:8" x14ac:dyDescent="0.3">
@@ -12193,8 +12189,8 @@
       <c r="G303" t="s">
         <v>903</v>
       </c>
-      <c r="H303" s="3" t="s">
-        <v>1273</v>
+      <c r="H303" t="s">
+        <v>1272</v>
       </c>
     </row>
     <row r="304" spans="1:8" x14ac:dyDescent="0.3">
@@ -12219,8 +12215,8 @@
       <c r="G304" t="s">
         <v>904</v>
       </c>
-      <c r="H304" s="3" t="s">
-        <v>1274</v>
+      <c r="H304" t="s">
+        <v>1273</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.3">
@@ -12245,8 +12241,8 @@
       <c r="G305" t="s">
         <v>905</v>
       </c>
-      <c r="H305" s="3" t="s">
-        <v>1275</v>
+      <c r="H305" t="s">
+        <v>1274</v>
       </c>
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.3">
@@ -12271,8 +12267,8 @@
       <c r="G306" t="s">
         <v>906</v>
       </c>
-      <c r="H306" s="3" t="s">
-        <v>1276</v>
+      <c r="H306" t="s">
+        <v>1275</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.3">
@@ -12297,8 +12293,8 @@
       <c r="G307" t="s">
         <v>904</v>
       </c>
-      <c r="H307" s="3" t="s">
-        <v>1277</v>
+      <c r="H307" t="s">
+        <v>1276</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.3">
@@ -12323,8 +12319,8 @@
       <c r="G308" t="s">
         <v>905</v>
       </c>
-      <c r="H308" s="3" t="s">
-        <v>1278</v>
+      <c r="H308" t="s">
+        <v>1277</v>
       </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.3">
@@ -12349,8 +12345,8 @@
       <c r="G309" t="s">
         <v>907</v>
       </c>
-      <c r="H309" s="3" t="s">
-        <v>1279</v>
+      <c r="H309" t="s">
+        <v>1278</v>
       </c>
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.3">
@@ -12375,8 +12371,8 @@
       <c r="G310" t="s">
         <v>908</v>
       </c>
-      <c r="H310" s="3" t="s">
-        <v>1280</v>
+      <c r="H310" t="s">
+        <v>1279</v>
       </c>
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.3">
@@ -12401,8 +12397,8 @@
       <c r="G311" t="s">
         <v>909</v>
       </c>
-      <c r="H311" s="3" t="s">
-        <v>1281</v>
+      <c r="H311" t="s">
+        <v>1280</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.3">
@@ -12427,8 +12423,8 @@
       <c r="G312" t="s">
         <v>904</v>
       </c>
-      <c r="H312" s="3" t="s">
-        <v>1282</v>
+      <c r="H312" t="s">
+        <v>1281</v>
       </c>
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.3">
@@ -12453,8 +12449,8 @@
       <c r="G313" t="s">
         <v>904</v>
       </c>
-      <c r="H313" s="3" t="s">
-        <v>1283</v>
+      <c r="H313" t="s">
+        <v>1282</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.3">
@@ -12479,8 +12475,8 @@
       <c r="G314" t="s">
         <v>99</v>
       </c>
-      <c r="H314" s="3" t="s">
-        <v>1284</v>
+      <c r="H314" t="s">
+        <v>1283</v>
       </c>
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.3">
@@ -12505,8 +12501,8 @@
       <c r="G315" t="s">
         <v>334</v>
       </c>
-      <c r="H315" s="3" t="s">
-        <v>1285</v>
+      <c r="H315" t="s">
+        <v>1284</v>
       </c>
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.3">
@@ -12531,8 +12527,8 @@
       <c r="G316" t="s">
         <v>910</v>
       </c>
-      <c r="H316" s="3" t="s">
-        <v>1286</v>
+      <c r="H316" t="s">
+        <v>1285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>